<commit_message>
Added the relative path
</commit_message>
<xml_diff>
--- a/Demo_smart_hospital/ExcelReader/NewPatientData.xlsx
+++ b/Demo_smart_hospital/ExcelReader/NewPatientData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pytest_Mainproject\pilot_project_Demo_smart_hospital_Pytest\Demo_smart_hospital\ExcelReader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dinesh_branch_pytest_demo_smart_hospital\pilot_project_Demo_smart_hospital_Pytest\Demo_smart_hospital\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27BC60B-1061-49AA-B543-5BB54BEB32F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CD7FE6-4B13-4B03-ADCD-328EDED16A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1F9BC631-AE66-45E6-AEC9-5DC2ED437C72}"/>
+    <workbookView xWindow="312" yWindow="2784" windowWidth="17280" windowHeight="8880" xr2:uid="{1F9BC631-AE66-45E6-AEC9-5DC2ED437C72}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_data" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>kowshik</t>
-  </si>
-  <si>
-    <t>kowshikkrishnan@gmail.com</t>
+    <t>sweatha</t>
+  </si>
+  <si>
+    <t>sweatha@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -165,18 +165,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,26 +467,26 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="18.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -539,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -556,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <v>9876545673</v>
+        <v>9345265655</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>23</v>
@@ -596,12 +584,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -642,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>